<commit_message>
Update : multiple file export by sheet name
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="app" sheetId="1" r:id="rId1"/>
+    <sheet name="other" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>EN</t>
   </si>
@@ -91,6 +91,57 @@
   </si>
   <si>
     <t>ARKEY5</t>
+  </si>
+  <si>
+    <t>EN OTHER 2</t>
+  </si>
+  <si>
+    <t>EN OTHER 3</t>
+  </si>
+  <si>
+    <t>EN OTHER 4</t>
+  </si>
+  <si>
+    <t>EN OTHER 5</t>
+  </si>
+  <si>
+    <t>ID OTHER 2</t>
+  </si>
+  <si>
+    <t>ID OTHER 3</t>
+  </si>
+  <si>
+    <t>ID OTHER 4</t>
+  </si>
+  <si>
+    <t>ID OTHER 5</t>
+  </si>
+  <si>
+    <t>AR OTHER 2</t>
+  </si>
+  <si>
+    <t>AR OTHER 3</t>
+  </si>
+  <si>
+    <t>AR OTHER 4</t>
+  </si>
+  <si>
+    <t>AR OTHER 5</t>
+  </si>
+  <si>
+    <t>OTHER1</t>
+  </si>
+  <si>
+    <t>OTHER2</t>
+  </si>
+  <si>
+    <t>OTHER3</t>
+  </si>
+  <si>
+    <t>OTHER4</t>
+  </si>
+  <si>
+    <t>OTHER5</t>
   </si>
 </sst>
 </file>
@@ -502,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,13 +666,117 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="4" width="26.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>